<commit_message>
xlbh anh tuan BG
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang5/2.XulyBH/XLBH2205_AnhTuanBG.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang5/2.XulyBH/XLBH2205_AnhTuanBG.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="4035" windowWidth="10320" windowHeight="4065" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="4035" windowWidth="10320" windowHeight="4065"/>
   </bookViews>
   <sheets>
     <sheet name="TG102V" sheetId="43" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="108">
   <si>
     <t>STT</t>
   </si>
@@ -330,7 +330,37 @@
     <t>Hết hạn dịch vụ</t>
   </si>
   <si>
-    <t>Sim lỗi</t>
+    <t>LE.1.00.---05.190404</t>
+  </si>
+  <si>
+    <t>Thiết bị dấu hiệu nước vào oxi hóa nặng</t>
+  </si>
+  <si>
+    <t>Không sửa chữa</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>Sim lỗi, hết hạn dịch vụ</t>
+  </si>
+  <si>
+    <t>W.2.00.---21.200630</t>
+  </si>
+  <si>
+    <t>VI.2.00.---19.200527</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W.1.00.---01.181101 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">W.1.00.---01.180629 </t>
+  </si>
+  <si>
+    <t>VI.2.00.---21.200630</t>
+  </si>
+  <si>
+    <t>Nâng cấp khay sim, nâng cấp FW</t>
   </si>
 </sst>
 </file>
@@ -1060,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1288,9 +1318,13 @@
         <v>79</v>
       </c>
       <c r="H6" s="37"/>
-      <c r="I6" s="51"/>
+      <c r="I6" s="51" t="s">
+        <v>84</v>
+      </c>
       <c r="J6" s="1"/>
-      <c r="K6" s="55"/>
+      <c r="K6" s="55" t="s">
+        <v>103</v>
+      </c>
       <c r="L6" s="39"/>
       <c r="M6" s="39"/>
       <c r="N6" s="1"/>
@@ -1322,21 +1356,39 @@
       <c r="E7" s="38">
         <v>863586032908760</v>
       </c>
-      <c r="F7" s="37"/>
+      <c r="F7" s="37" t="s">
+        <v>80</v>
+      </c>
       <c r="G7" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="H7" s="47"/>
-      <c r="I7" s="51"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="51" t="s">
+        <v>84</v>
+      </c>
       <c r="J7" s="1"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
+      <c r="K7" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="M7" s="39" t="s">
+        <v>107</v>
+      </c>
       <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="2"/>
+      <c r="O7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P7" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="S7" s="3"/>
       <c r="T7" s="58"/>
       <c r="U7" s="62"/>
@@ -1359,21 +1411,41 @@
       <c r="E8" s="38">
         <v>864811036929946</v>
       </c>
-      <c r="F8" s="37"/>
+      <c r="F8" s="37" t="s">
+        <v>80</v>
+      </c>
       <c r="G8" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="51"/>
+      <c r="H8" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="I8" s="51" t="s">
+        <v>84</v>
+      </c>
       <c r="J8" s="1"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
+      <c r="K8" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="L8" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="M8" s="39" t="s">
+        <v>107</v>
+      </c>
       <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="2"/>
+      <c r="O8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P8" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="S8" s="3"/>
       <c r="T8" s="58"/>
       <c r="U8" s="62"/>
@@ -1401,16 +1473,32 @@
         <v>79</v>
       </c>
       <c r="H9" s="37"/>
-      <c r="I9" s="51"/>
+      <c r="I9" s="51" t="s">
+        <v>84</v>
+      </c>
       <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
+      <c r="K9" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L9" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="M9" s="39" t="s">
+        <v>107</v>
+      </c>
       <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="2"/>
+      <c r="O9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P9" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="S9" s="3"/>
       <c r="T9" s="58"/>
       <c r="U9" s="62"/>
@@ -1437,17 +1525,35 @@
       <c r="G10" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="H10" s="47"/>
-      <c r="I10" s="51"/>
+      <c r="H10" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="I10" s="51" t="s">
+        <v>84</v>
+      </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
+      <c r="K10" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="L10" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="M10" s="39" t="s">
+        <v>107</v>
+      </c>
       <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="2"/>
+      <c r="O10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P10" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="S10" s="3"/>
       <c r="T10" s="58"/>
       <c r="U10" s="62"/>
@@ -1808,7 +1914,7 @@
       </c>
       <c r="V22" s="9">
         <f>COUNTIF($Q$6:$Q$51,"PC+PM")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W22" s="13"/>
     </row>
@@ -2085,7 +2191,7 @@
       </c>
       <c r="V31" s="9">
         <f>COUNTIF($R$6:$R$51,"*LK*")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W31" s="13"/>
     </row>
@@ -2213,7 +2319,7 @@
       </c>
       <c r="V35" s="9">
         <f>COUNTIF($R$6:$R$51,"*NCFW*")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W35" s="13"/>
     </row>
@@ -2277,7 +2383,7 @@
       </c>
       <c r="V37" s="9">
         <f>SUM(V26:V36)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W37" s="13"/>
     </row>
@@ -3342,13 +3448,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -3360,6 +3459,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3370,8 +3476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X115"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3824,7 +3930,7 @@
         <v>79</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="I10" s="51" t="s">
         <v>84</v>
@@ -3833,13 +3939,25 @@
       <c r="K10" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
+      <c r="L10" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="M10" s="39" t="s">
+        <v>38</v>
+      </c>
       <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="2"/>
+      <c r="O10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P10" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="S10" s="3"/>
       <c r="T10" s="58"/>
       <c r="U10" s="62"/>
@@ -3867,16 +3985,32 @@
         <v>79</v>
       </c>
       <c r="H11" s="60"/>
-      <c r="I11" s="51"/>
+      <c r="I11" s="51" t="s">
+        <v>84</v>
+      </c>
       <c r="J11" s="1"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
+      <c r="K11" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="L11" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="M11" s="39" t="s">
+        <v>38</v>
+      </c>
       <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="2"/>
+      <c r="O11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P11" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="S11" s="3"/>
       <c r="T11" s="58"/>
       <c r="U11" s="62"/>
@@ -3904,16 +4038,32 @@
         <v>79</v>
       </c>
       <c r="H12" s="60"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
+      <c r="I12" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K12" s="55"/>
+      <c r="L12" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="M12" s="39" t="s">
+        <v>94</v>
+      </c>
       <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="2"/>
+      <c r="O12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P12" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="S12" s="3"/>
       <c r="T12" s="58"/>
       <c r="U12" s="61" t="s">
@@ -3944,15 +4094,27 @@
       </c>
       <c r="H13" s="47"/>
       <c r="I13" s="51"/>
-      <c r="J13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="K13" s="1"/>
       <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
+      <c r="M13" s="39" t="s">
+        <v>99</v>
+      </c>
       <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="2"/>
+      <c r="O13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P13" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="S13" s="3"/>
       <c r="T13" s="58"/>
       <c r="U13" s="62"/>
@@ -4160,7 +4322,7 @@
       </c>
       <c r="V20" s="9">
         <f>COUNTIF($Q$6:$Q$51,"PM")</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="W20" s="13"/>
     </row>
@@ -4192,7 +4354,7 @@
       </c>
       <c r="V21" s="9">
         <f>COUNTIF($Q$6:$Q$51,"PC")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W21" s="13"/>
     </row>
@@ -4501,7 +4663,7 @@
       </c>
       <c r="V31" s="9">
         <f>COUNTIF($R$6:$R$51,"*LK*")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W31" s="13"/>
     </row>
@@ -4533,7 +4695,7 @@
       </c>
       <c r="V32" s="9">
         <f>COUNTIF($R$6:$R$51,"*MCH*")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W32" s="13"/>
     </row>
@@ -4629,7 +4791,7 @@
       </c>
       <c r="V35" s="9">
         <f>COUNTIF($R$6:$R$51,"*NCFW*")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W35" s="13"/>
     </row>
@@ -4693,7 +4855,7 @@
       </c>
       <c r="V37" s="9">
         <f>SUM(V26:V36)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="W37" s="13"/>
     </row>
@@ -4811,7 +4973,7 @@
       </c>
       <c r="V41" s="9">
         <f>COUNTIF($O$6:$O$51,"*KS*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W41" s="13"/>
     </row>
@@ -5758,13 +5920,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -5776,6 +5931,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8094,6 +8256,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -8105,13 +8274,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9879,6 +10041,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -9890,13 +10059,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>